<commit_message>
Change Q1 to IRLML6344TRPBF.
</commit_message>
<xml_diff>
--- a/aaXBee_BOM.xlsx
+++ b/aaXBee_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="18195" windowHeight="13110" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="18195" windowHeight="13110"/>
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="274">
   <si>
     <t>Mouser #</t>
   </si>
@@ -186,18 +186,9 @@
     <t>Thick Film Resistors - SMD 1/8watts 2.2Kohms 1%</t>
   </si>
   <si>
-    <t>942-IRLML6244TRPBF</t>
-  </si>
-  <si>
-    <t>IRLML6244TRPBF</t>
-  </si>
-  <si>
     <t>International Rectifier</t>
   </si>
   <si>
-    <t>MOSFET MOSFT 20V 6.3A 21mOhm 2.5V cpbl</t>
-  </si>
-  <si>
     <t>604-APT2012YC</t>
   </si>
   <si>
@@ -648,9 +639,6 @@
     <t>L3</t>
   </si>
   <si>
-    <t>IRLML6244TR</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -847,6 +835,15 @@
   </si>
   <si>
     <t>Optional components, X = required.</t>
+  </si>
+  <si>
+    <t>IRLML6344TRPBF</t>
+  </si>
+  <si>
+    <t>942-IRLML6344TRPBF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET MOSFT 5.0A 29mOhm 30V 2.5V drv capable </t>
   </si>
 </sst>
 </file>
@@ -1353,7 +1350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1367,25 +1364,25 @@
   <sheetData>
     <row r="1" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -1405,19 +1402,19 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" t="s">
         <v>102</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1425,19 +1422,19 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" t="s">
         <v>148</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="E7" t="s">
-        <v>150</v>
-      </c>
-      <c r="F7" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1445,19 +1442,19 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D8" s="9">
         <v>2462</v>
       </c>
       <c r="E8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1465,19 +1462,19 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" t="s">
         <v>91</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1485,19 +1482,19 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" t="s">
         <v>95</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F10" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1505,19 +1502,19 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" t="s">
         <v>83</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E11" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1525,19 +1522,19 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" t="s">
         <v>87</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" t="s">
-        <v>89</v>
-      </c>
-      <c r="F12" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1545,19 +1542,19 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" t="s">
         <v>79</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1565,19 +1562,19 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" t="s">
         <v>75</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1585,19 +1582,19 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1605,19 +1602,19 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1625,19 +1622,19 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" t="s">
         <v>58</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1645,19 +1642,19 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" t="s">
         <v>68</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1665,19 +1662,19 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1685,19 +1682,19 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C20" t="s">
+        <v>272</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="E20" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" t="s">
-        <v>56</v>
-      </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1705,7 +1702,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
@@ -1725,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C22" t="s">
         <v>33</v>
@@ -1745,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C23" t="s">
         <v>30</v>
@@ -1765,7 +1762,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
         <v>27</v>
@@ -1785,7 +1782,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
@@ -1805,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C26" t="s">
         <v>45</v>
@@ -1825,7 +1822,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C27" t="s">
         <v>51</v>
@@ -1845,7 +1842,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C28" t="s">
         <v>42</v>
@@ -1865,7 +1862,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
@@ -1885,7 +1882,7 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C30" t="s">
         <v>36</v>
@@ -1905,7 +1902,7 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C31" t="s">
         <v>19</v>
@@ -1925,7 +1922,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C32" t="s">
         <v>16</v>
@@ -1945,7 +1942,7 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
@@ -1965,7 +1962,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
@@ -1985,19 +1982,19 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C35" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E35" t="s">
         <v>6</v>
       </c>
       <c r="F35" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2005,7 +2002,7 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -2025,19 +2022,19 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C37" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37" t="s">
         <v>106</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E37" t="s">
-        <v>108</v>
-      </c>
-      <c r="F37" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2056,9 +2053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2080,33 +2075,33 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" t="s">
         <v>158</v>
       </c>
-      <c r="B5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D5" t="s">
-        <v>157</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H5" t="s">
         <v>160</v>
-      </c>
-      <c r="F5" t="s">
-        <v>161</v>
-      </c>
-      <c r="G5" t="s">
-        <v>162</v>
-      </c>
-      <c r="H5" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2114,25 +2109,25 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2140,25 +2135,25 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2166,25 +2161,25 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2203,7 +2198,7 @@
   </sheetPr>
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2226,1156 +2221,1156 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>208</v>
+        <v>271</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B43" s="6">
         <v>220</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C51" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>242</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F56" s="5"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F61" s="5"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B63" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B68" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B71" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>